<commit_message>
Dumb and Dumber To
Almost fully coded
</commit_message>
<xml_diff>
--- a/_03_part-two/movies/film-details-and-ids.xlsx
+++ b/_03_part-two/movies/film-details-and-ids.xlsx
@@ -5,14 +5,14 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\James\Documents\GitHub\COGS187AFinalProject\_03_part-two\movies\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GitHub\COGS187AFinalProject\_03_part-two\movies\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="600" windowWidth="28800" windowHeight="12420"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Playing Now" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,12 +24,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>ID</t>
   </si>
   <si>
     <t>Film Name</t>
+  </si>
+  <si>
+    <t>Genre</t>
   </si>
 </sst>
 </file>
@@ -347,21 +350,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="13.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>